<commit_message>
Adding a way to provide locale and translations from the server as part of the data loaded from the excel template.
</commit_message>
<xml_diff>
--- a/quote-generator-prototype/resources/public/import/quote-generator-template.xlsx
+++ b/quote-generator-prototype/resources/public/import/quote-generator-template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
   <si>
     <t>id</t>
   </si>
@@ -134,13 +134,19 @@
     <t>I18n</t>
   </si>
   <si>
-    <t>English</t>
+    <t>Translation</t>
+  </si>
+  <si>
+    <t>Locale</t>
   </si>
   <si>
     <t>LoginTitle</t>
   </si>
   <si>
     <t>Login title goes here</t>
+  </si>
+  <si>
+    <t>en-US</t>
   </si>
   <si>
     <t>LoginSubtitle</t>
@@ -769,277 +775,382 @@
       <c r="B1" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="36">
@@ -3951,7 +4062,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Pushing translations to the server and changing the client to load them.
</commit_message>
<xml_diff>
--- a/quote-generator-prototype/resources/public/import/quote-generator-template.xlsx
+++ b/quote-generator-prototype/resources/public/import/quote-generator-template.xlsx
@@ -170,7 +170,15 @@
     <t>HomeDescription</t>
   </si>
   <si>
-    <t>A Quote is a list of Products.\nA Product is made up of Features.\nEach Product has a set of Base Features, which are mandatory.\nEach Product has a set of Additional Features, which are optional.\n\nUse the Products button to go to the list of products.\nSelect a Product to view it's Features. Additional Features may be added through the Quantity input. When you have the Product in the desired state, use the Add to Quote button to add it to your Quote. You will then be brought to the Quote Summary page.\n\nThe Quote Summary is like a shopping cart for the Products you want to create a Quote for. At any point, you can see what is in the existing Quote by clicking on the Quote Summary button. If you want to add more Products, use the Product button to go back to the list of products. If you want to remove a Product, use the X button to the right of the Product's Cost.\n\nWhen you have what you need in the Quote, Submit the Quote from the Quote Summary page.\n\nThese instructions are always available by clicking on the logo in the header as well as the Help button.</t>
+    <t>A Quote is a list of Products.
+A Product is made up of Features.
+Each Product has a set of Base Features, which are mandatory.
+Each Product has a set of Additional Features, which are optional.
+Use the Products button to go to the list of products.
+Select a Product to view it's Features. Additional Features may be added through the Quantity input. When you have the Product in the desired state, use the Add to Quote button to add it to your Quote. You will then be brought to the Quote Summary page.
+The Quote Summary is like a shopping cart for the Products you want to create a Quote for. At any point, you can see what is in the existing Quote by clicking on the Quote Summary button. If you want to add more Products, use the Product button to go back to the list of products. If you want to remove a Product, use the X button to the right of the Product's Cost.
+When you have what you need in the Quote, Submit the Quote from the Quote Summary page.
+These instructions are always available by clicking on the logo in the header as well as the Help button.</t>
   </si>
   <si>
     <t>NavigateToProductCatalog</t>

</xml_diff>